<commit_message>
Consultar com filtro feita
</commit_message>
<xml_diff>
--- a/Analise/Excel/ExcelTCC.xlsx
+++ b/Analise/Excel/ExcelTCC.xlsx
@@ -3,21 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBA45B0-B418-4FC7-ACAF-E2144C9F679A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4B70A1-FBAE-43F7-826D-5FC300DD06E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Casos de uso</t>
   </si>
@@ -104,6 +102,9 @@
   </si>
   <si>
     <t>1ª Semana até dia 12/10</t>
+  </si>
+  <si>
+    <t>Tela esqueci a senha</t>
   </si>
 </sst>
 </file>
@@ -145,7 +146,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -214,6 +215,15 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top/>
       <bottom style="medium">
@@ -237,7 +247,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,7 +589,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,10 +700,10 @@
       <c r="B6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="11" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -704,35 +714,13 @@
       <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11"/>
+      <c r="C7" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Consultando Se O Anuncio Esta Favoritado
</commit_message>
<xml_diff>
--- a/Analise/Excel/ExcelTCC.xlsx
+++ b/Analise/Excel/ExcelTCC.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024600F0-7FE2-4A03-A4F0-2BF7621D9777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26CCFCE-0D15-4955-8FB9-522DB5080583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -104,7 +104,7 @@
     <t>Tela Home com anuncios com consulta ou sem consulta e filtro</t>
   </si>
   <si>
-    <t>Backend consultar um anuncio favorito</t>
+    <t>Backend consultar se o anuncio esta favoritado</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -259,6 +259,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -601,7 +604,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,8 +738,8 @@
       </c>
       <c r="F9" s="11"/>
     </row>
-    <row r="10" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="4" t="s">
+    <row r="10" spans="1:6" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="14" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="11"/>

</xml_diff>